<commit_message>
uploaded from Matlab using gitUpload()
</commit_message>
<xml_diff>
--- a/lesions.xlsx
+++ b/lesions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="26940" windowHeight="12915"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="26940" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>'Naty388'</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Naty341'</t>
+  </si>
+  <si>
+    <t>TryskoMys</t>
+  </si>
+  <si>
+    <t>Naty338</t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,6 +521,9 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
       <c r="C4">
         <v>283</v>
       </c>
@@ -598,6 +607,9 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
       </c>
       <c r="C7">
         <v>338</v>

</xml_diff>

<commit_message>
Uploaded from Matlab using gitup()
</commit_message>
<xml_diff>
--- a/lesions.xlsx
+++ b/lesions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="26940" windowHeight="12915"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="26940" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>FR</t>
   </si>
   <si>
-    <t>SkullFluoro</t>
-  </si>
-  <si>
     <t>PremekMysFinal</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>Naty338</t>
+  </si>
+  <si>
+    <t>SkullFluoro_mm2</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +456,7 @@
         <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -464,7 +464,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>339</v>
@@ -493,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>419</v>
@@ -522,7 +522,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>283</v>
@@ -551,7 +551,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>343</v>
@@ -580,7 +580,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>413</v>
@@ -609,7 +609,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>338</v>
@@ -638,7 +638,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>341</v>

</xml_diff>